<commit_message>
Save changes before rebase
</commit_message>
<xml_diff>
--- a/LubanConfig/MiniTemplate/Datas/monster.xlsx
+++ b/LubanConfig/MiniTemplate/Datas/monster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Mota\LubanConfig\MiniTemplate\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5399E220-FD82-4524-B561-47C57CF30F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD138E57-EA28-4840-B041-E21DAF609800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="2850" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,14 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>icon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圖標</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*items</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,6 +197,22 @@
   </si>
   <si>
     <t>無</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>動畫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -595,7 +603,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -619,23 +627,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -646,26 +654,26 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,166 +687,183 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
         <v>42</v>
       </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
       <c r="I10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>